<commit_message>
New locations added with the tree count
</commit_message>
<xml_diff>
--- a/data/Locations.xlsx
+++ b/data/Locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\landscapingUOB-api\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987782EE-D95A-4BB2-92A9-797EF58C3F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABA6806-F7A0-43E5-B201-8F5DA79F404C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="137">
   <si>
     <t>Location type</t>
   </si>
@@ -426,6 +426,27 @@
   </si>
   <si>
     <t>Location Number</t>
+  </si>
+  <si>
+    <t>Car park</t>
+  </si>
+  <si>
+    <t>Running Track</t>
+  </si>
+  <si>
+    <t>Residential</t>
+  </si>
+  <si>
+    <t>Villas</t>
+  </si>
+  <si>
+    <t>Roadside</t>
+  </si>
+  <si>
+    <t>Internal Ring Road</t>
+  </si>
+  <si>
+    <t>Trees quantity</t>
   </si>
 </sst>
 </file>
@@ -461,7 +482,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -471,6 +492,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE163"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -488,7 +527,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -506,23 +545,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -798,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="131" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -815,7 +855,7 @@
     <col min="8" max="8" width="15.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -828,8 +868,11 @@
       <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -842,8 +885,11 @@
       <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -856,8 +902,11 @@
       <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -870,8 +919,11 @@
       <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -884,8 +936,11 @@
       <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E5">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -898,8 +953,11 @@
       <c r="D6" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E6">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -912,8 +970,11 @@
       <c r="D7" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E7">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -926,8 +987,11 @@
       <c r="D8" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E8">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -940,8 +1004,11 @@
       <c r="D9" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E9">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -954,8 +1021,11 @@
       <c r="D10" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -968,8 +1038,11 @@
       <c r="D11" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E11">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -982,8 +1055,11 @@
       <c r="D12" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E12">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -996,8 +1072,11 @@
       <c r="D13" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E13">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1010,8 +1089,11 @@
       <c r="D14" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E14">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1024,8 +1106,11 @@
       <c r="D15" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E15">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1038,8 +1123,11 @@
       <c r="D16" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E16">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1052,8 +1140,11 @@
       <c r="D17" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E17">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1066,22 +1157,28 @@
       <c r="D18" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="E18">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E19" s="7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -1094,8 +1191,11 @@
       <c r="D20" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E20">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -1108,8 +1208,11 @@
       <c r="D21" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E21">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1122,8 +1225,11 @@
       <c r="D22" s="5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E22">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1136,8 +1242,11 @@
       <c r="D23" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E23">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -1150,8 +1259,11 @@
       <c r="D24" s="5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E24">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -1164,8 +1276,11 @@
       <c r="D25" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -1178,8 +1293,11 @@
       <c r="D26" s="5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E26">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -1192,22 +1310,25 @@
       <c r="D27" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="E27">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -1220,8 +1341,11 @@
       <c r="D29" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E29">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1234,8 +1358,11 @@
       <c r="D30" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E30">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -1248,8 +1375,11 @@
       <c r="D31" s="5" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E31">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -1262,8 +1392,11 @@
       <c r="D32" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E32">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -1276,50 +1409,62 @@
       <c r="D33" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="E33">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="8" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="E34" s="7">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="8" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>3</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="E35" s="7">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E36" s="7">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -1332,8 +1477,11 @@
       <c r="D37" s="5" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E37">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>111</v>
       </c>
@@ -1346,119 +1494,300 @@
       <c r="D38" s="5" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E38">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>115</v>
       </c>
       <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" t="s">
+        <v>131</v>
+      </c>
+      <c r="D39" s="9"/>
+      <c r="E39">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D40" s="8" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>119</v>
-      </c>
-      <c r="B40" t="s">
-        <v>120</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E40" s="7">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>119</v>
       </c>
       <c r="B41" t="s">
-        <v>123</v>
-      </c>
-      <c r="C41" t="s">
-        <v>124</v>
+        <v>120</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+      <c r="E41">
+        <v>5300</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>119</v>
       </c>
       <c r="B42" t="s">
+        <v>123</v>
+      </c>
+      <c r="C42" t="s">
+        <v>124</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E42">
+        <v>16500</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B43" t="s">
         <v>126</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>127</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D43" s="5" t="s">
         <v>128</v>
       </c>
+      <c r="E43">
+        <v>16500</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>130</v>
+      </c>
+      <c r="B44" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>130</v>
+      </c>
+      <c r="B45" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" t="s">
+        <v>53</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E45">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E46" s="7">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>130</v>
+      </c>
+      <c r="B47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" t="s">
+        <v>62</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E47">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>130</v>
+      </c>
+      <c r="B48" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E48">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>130</v>
+      </c>
+      <c r="B49" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49" t="s">
+        <v>83</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E49">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>130</v>
+      </c>
+      <c r="B50" t="s">
+        <v>126</v>
+      </c>
+      <c r="C50" t="s">
+        <v>127</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E50">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>132</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" t="s">
+        <v>133</v>
+      </c>
+      <c r="D51" s="10"/>
+      <c r="E51">
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>134</v>
+      </c>
+      <c r="B52" s="11"/>
+      <c r="C52" t="s">
+        <v>135</v>
+      </c>
+      <c r="D52" s="10"/>
+      <c r="E52">
+        <v>13500</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D42">
-    <sortCondition ref="A2:A42"/>
-    <sortCondition ref="B2:B42"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D43">
+    <sortCondition ref="A2:A43"/>
+    <sortCondition ref="B2:B43"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{12928F6E-5312-4F47-8E2A-2DA233330493}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A41:A1048576 A2:A39" xr:uid="{12928F6E-5312-4F47-8E2A-2DA233330493}">
       <formula1>"Building,Gate,Roadside,Residential,Infrastructure,Facilities,Car park"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1" xr:uid="{80EE9128-EF22-45E1-A050-B4A922D7A5A4}"/>
-    <hyperlink ref="D22" r:id="rId2" xr:uid="{6E85802D-CC4C-4BD4-83ED-55100DE115BA}"/>
-    <hyperlink ref="D25" r:id="rId3" xr:uid="{CA6F2ACE-9B39-4D45-9C20-19A5DB6D12CA}"/>
-    <hyperlink ref="D15" r:id="rId4" xr:uid="{892A1EEC-B028-4BF1-ADCD-AF96A0988B50}"/>
-    <hyperlink ref="D10" r:id="rId5" xr:uid="{F1426B06-7CBB-4D59-AE83-B095FA6474E2}"/>
-    <hyperlink ref="D8" r:id="rId6" xr:uid="{592D78FC-336C-471A-91BD-1562E94DA284}"/>
-    <hyperlink ref="D9" r:id="rId7" xr:uid="{A2D386D9-0502-4921-BB61-A819FF837370}"/>
-    <hyperlink ref="D19" r:id="rId8" xr:uid="{7BE3DA68-E823-4B16-885B-945823145A4E}"/>
-    <hyperlink ref="D13" r:id="rId9" xr:uid="{5A89EF2A-F868-480F-9E72-4F25C74088A4}"/>
-    <hyperlink ref="D31" r:id="rId10" xr:uid="{99947C2E-DEFB-4F3D-B10B-4C51E1A36A2A}"/>
-    <hyperlink ref="D33" r:id="rId11" xr:uid="{8D11C5C3-9012-49EE-A7E5-072DFCD7E4CB}"/>
-    <hyperlink ref="D2" r:id="rId12" xr:uid="{6CF4DEC1-CD4E-4844-A06E-A3B5553E4A0A}"/>
-    <hyperlink ref="D3" r:id="rId13" xr:uid="{9E806015-46CC-43F4-B15B-0F80E18DD0D3}"/>
-    <hyperlink ref="D4" r:id="rId14" xr:uid="{0BE1B822-D34C-40EF-8B0F-F98C95A68F23}"/>
-    <hyperlink ref="D11" r:id="rId15" xr:uid="{BD02D7C7-CF92-4415-BD68-A5E1CD860AB5}"/>
-    <hyperlink ref="D16" r:id="rId16" xr:uid="{B21EE433-AA31-44F8-A2B5-B896D27134D4}"/>
-    <hyperlink ref="D14" r:id="rId17" xr:uid="{E2D6E56A-BEDF-4371-A57A-AE46E0B0D271}"/>
-    <hyperlink ref="D17" r:id="rId18" xr:uid="{6EEDF604-934E-4BBF-844F-1CBB5949AF7F}"/>
-    <hyperlink ref="D18" r:id="rId19" xr:uid="{2D6E9249-18AB-4397-B0F5-437EFBC6F332}"/>
-    <hyperlink ref="D36" r:id="rId20" xr:uid="{E63D41F9-5B08-43E0-8053-0724E6D37B6B}"/>
-    <hyperlink ref="D21" r:id="rId21" xr:uid="{5BA1C18C-D565-4734-9906-9C0A7DC7BFEA}"/>
-    <hyperlink ref="D27" r:id="rId22" xr:uid="{40D3F8D6-8B9A-4507-8102-4BFB0D9B2580}"/>
-    <hyperlink ref="D26" r:id="rId23" xr:uid="{EFEDD41E-1E02-461C-9393-AD2ACCBC2A60}"/>
-    <hyperlink ref="D32" r:id="rId24" xr:uid="{0BEBBA09-865C-426C-A4B4-4F2481A2A4E8}"/>
-    <hyperlink ref="D12" r:id="rId25" xr:uid="{9B82FEF9-0E16-4B92-A3E1-1FC2CB2AF171}"/>
-    <hyperlink ref="D7" r:id="rId26" xr:uid="{2ED0409A-8763-4061-A855-6C9AC6A9D6BD}"/>
-    <hyperlink ref="D28" r:id="rId27" xr:uid="{A6B3F117-56EC-4411-89C5-2B81B32C6D2F}"/>
-    <hyperlink ref="D29" r:id="rId28" xr:uid="{45AB639A-6A68-47E6-820F-5AE96EF37CCE}"/>
-    <hyperlink ref="D30" r:id="rId29" xr:uid="{7CB307A7-AD29-447B-B87B-FDF01946BA4A}"/>
-    <hyperlink ref="D24" r:id="rId30" xr:uid="{D83D9F73-94C9-4362-9F33-9764794F83C7}"/>
-    <hyperlink ref="D23" r:id="rId31" xr:uid="{13D49606-5D63-4601-9617-2606341647E2}"/>
-    <hyperlink ref="D34" r:id="rId32" xr:uid="{E93DF50E-6385-47B4-B2C7-B9246E51EFC3}"/>
-    <hyperlink ref="D39" r:id="rId33" xr:uid="{887D03B3-F5B5-4EC3-B378-CFF1ACACC697}"/>
-    <hyperlink ref="D40" r:id="rId34" xr:uid="{25328B39-D4E0-444C-9000-8F992DB7BA09}"/>
-    <hyperlink ref="D20" r:id="rId35" xr:uid="{80ECF8CD-7A79-402A-B5EC-F9BA63C3B50A}"/>
-    <hyperlink ref="D42" r:id="rId36" xr:uid="{6B7E0906-BF85-4BF1-A5E5-9F4F8AB12E12}"/>
-    <hyperlink ref="D41" r:id="rId37" xr:uid="{A757999D-BA12-4BC4-B318-11BE5E932894}"/>
-    <hyperlink ref="D38" r:id="rId38" xr:uid="{6AF44C4C-D5AE-4BD7-8C44-C3D0460467C0}"/>
-    <hyperlink ref="D35" r:id="rId39" xr:uid="{368C86F0-6C72-4FCF-9F6B-86FBA36B83AF}"/>
-    <hyperlink ref="D6" r:id="rId40" xr:uid="{705A06BF-AD9E-4AEF-8BEC-6580A15197D6}"/>
-    <hyperlink ref="D37" r:id="rId41" xr:uid="{6683E2F8-FB9A-4014-9996-7FEAAC683B93}"/>
+    <hyperlink ref="D25" r:id="rId2" xr:uid="{CA6F2ACE-9B39-4D45-9C20-19A5DB6D12CA}"/>
+    <hyperlink ref="D15" r:id="rId3" xr:uid="{892A1EEC-B028-4BF1-ADCD-AF96A0988B50}"/>
+    <hyperlink ref="D10" r:id="rId4" xr:uid="{F1426B06-7CBB-4D59-AE83-B095FA6474E2}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{592D78FC-336C-471A-91BD-1562E94DA284}"/>
+    <hyperlink ref="D9" r:id="rId6" xr:uid="{A2D386D9-0502-4921-BB61-A819FF837370}"/>
+    <hyperlink ref="D19" r:id="rId7" xr:uid="{7BE3DA68-E823-4B16-885B-945823145A4E}"/>
+    <hyperlink ref="D13" r:id="rId8" xr:uid="{5A89EF2A-F868-480F-9E72-4F25C74088A4}"/>
+    <hyperlink ref="D31" r:id="rId9" xr:uid="{99947C2E-DEFB-4F3D-B10B-4C51E1A36A2A}"/>
+    <hyperlink ref="D33" r:id="rId10" xr:uid="{8D11C5C3-9012-49EE-A7E5-072DFCD7E4CB}"/>
+    <hyperlink ref="D2" r:id="rId11" xr:uid="{6CF4DEC1-CD4E-4844-A06E-A3B5553E4A0A}"/>
+    <hyperlink ref="D3" r:id="rId12" xr:uid="{9E806015-46CC-43F4-B15B-0F80E18DD0D3}"/>
+    <hyperlink ref="D4" r:id="rId13" xr:uid="{0BE1B822-D34C-40EF-8B0F-F98C95A68F23}"/>
+    <hyperlink ref="D11" r:id="rId14" xr:uid="{BD02D7C7-CF92-4415-BD68-A5E1CD860AB5}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{B21EE433-AA31-44F8-A2B5-B896D27134D4}"/>
+    <hyperlink ref="D14" r:id="rId16" xr:uid="{E2D6E56A-BEDF-4371-A57A-AE46E0B0D271}"/>
+    <hyperlink ref="D17" r:id="rId17" xr:uid="{6EEDF604-934E-4BBF-844F-1CBB5949AF7F}"/>
+    <hyperlink ref="D18" r:id="rId18" xr:uid="{2D6E9249-18AB-4397-B0F5-437EFBC6F332}"/>
+    <hyperlink ref="D36" r:id="rId19" xr:uid="{E63D41F9-5B08-43E0-8053-0724E6D37B6B}"/>
+    <hyperlink ref="D21" r:id="rId20" xr:uid="{5BA1C18C-D565-4734-9906-9C0A7DC7BFEA}"/>
+    <hyperlink ref="D27" r:id="rId21" xr:uid="{40D3F8D6-8B9A-4507-8102-4BFB0D9B2580}"/>
+    <hyperlink ref="D26" r:id="rId22" xr:uid="{EFEDD41E-1E02-461C-9393-AD2ACCBC2A60}"/>
+    <hyperlink ref="D32" r:id="rId23" xr:uid="{0BEBBA09-865C-426C-A4B4-4F2481A2A4E8}"/>
+    <hyperlink ref="D12" r:id="rId24" xr:uid="{9B82FEF9-0E16-4B92-A3E1-1FC2CB2AF171}"/>
+    <hyperlink ref="D7" r:id="rId25" xr:uid="{2ED0409A-8763-4061-A855-6C9AC6A9D6BD}"/>
+    <hyperlink ref="D28" r:id="rId26" xr:uid="{A6B3F117-56EC-4411-89C5-2B81B32C6D2F}"/>
+    <hyperlink ref="D29" r:id="rId27" xr:uid="{45AB639A-6A68-47E6-820F-5AE96EF37CCE}"/>
+    <hyperlink ref="D30" r:id="rId28" xr:uid="{7CB307A7-AD29-447B-B87B-FDF01946BA4A}"/>
+    <hyperlink ref="D24" r:id="rId29" xr:uid="{D83D9F73-94C9-4362-9F33-9764794F83C7}"/>
+    <hyperlink ref="D23" r:id="rId30" xr:uid="{13D49606-5D63-4601-9617-2606341647E2}"/>
+    <hyperlink ref="D34" r:id="rId31" xr:uid="{E93DF50E-6385-47B4-B2C7-B9246E51EFC3}"/>
+    <hyperlink ref="D40" r:id="rId32" xr:uid="{887D03B3-F5B5-4EC3-B378-CFF1ACACC697}"/>
+    <hyperlink ref="D41" r:id="rId33" xr:uid="{25328B39-D4E0-444C-9000-8F992DB7BA09}"/>
+    <hyperlink ref="D20" r:id="rId34" xr:uid="{80ECF8CD-7A79-402A-B5EC-F9BA63C3B50A}"/>
+    <hyperlink ref="D43" r:id="rId35" xr:uid="{6B7E0906-BF85-4BF1-A5E5-9F4F8AB12E12}"/>
+    <hyperlink ref="D42" r:id="rId36" xr:uid="{A757999D-BA12-4BC4-B318-11BE5E932894}"/>
+    <hyperlink ref="D38" r:id="rId37" xr:uid="{6AF44C4C-D5AE-4BD7-8C44-C3D0460467C0}"/>
+    <hyperlink ref="D35" r:id="rId38" xr:uid="{368C86F0-6C72-4FCF-9F6B-86FBA36B83AF}"/>
+    <hyperlink ref="D6" r:id="rId39" xr:uid="{705A06BF-AD9E-4AEF-8BEC-6580A15197D6}"/>
+    <hyperlink ref="D37" r:id="rId40" xr:uid="{6683E2F8-FB9A-4014-9996-7FEAAC683B93}"/>
+    <hyperlink ref="D44" r:id="rId41" xr:uid="{F581F61C-236D-49A3-AE06-C2A7FF968C89}"/>
+    <hyperlink ref="D45" r:id="rId42" xr:uid="{BB91F514-736D-4FC9-A32E-788A20E577B9}"/>
+    <hyperlink ref="D46" r:id="rId43" xr:uid="{7EBDAD46-1A5B-4B2C-AF3D-61F18C3E275F}"/>
+    <hyperlink ref="D47" r:id="rId44" xr:uid="{A36D56AA-7C90-4154-A870-DA9409189D1F}"/>
+    <hyperlink ref="D22" r:id="rId45" xr:uid="{6E85802D-CC4C-4BD4-83ED-55100DE115BA}"/>
+    <hyperlink ref="D48" r:id="rId46" xr:uid="{00DDF648-5623-4E1D-8FC4-42D38FAEE4CA}"/>
+    <hyperlink ref="D49" r:id="rId47" xr:uid="{77EAAAD6-086C-4DCF-9B24-E59430A2E2FB}"/>
+    <hyperlink ref="D50" r:id="rId48" xr:uid="{CE8A3876-BF7A-4C23-95FB-161481F8F980}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Filter locations API by location number and type.
</commit_message>
<xml_diff>
--- a/data/Locations.xlsx
+++ b/data/Locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\landscapingUOB-api\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E250BD-CA42-4F4B-86E9-B88B6C81CB51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2E4F93-7D4A-411B-8D7B-5DFBCD163CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -840,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Test the Reports by adding a row that contains the year 2027.
</commit_message>
<xml_diff>
--- a/data/Locations.xlsx
+++ b/data/Locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\landscapingUOB-api\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2E4F93-7D4A-411B-8D7B-5DFBCD163CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FF441A-0007-4256-9878-A4489C1AB6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="136">
   <si>
     <t>Location type</t>
   </si>
@@ -432,9 +432,6 @@
   </si>
   <si>
     <t>Running Track</t>
-  </si>
-  <si>
-    <t>Residential</t>
   </si>
   <si>
     <t>Villas</t>
@@ -840,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -869,7 +866,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1702,13 +1699,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="B51" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C51" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D51" s="10"/>
       <c r="E51">
@@ -1717,11 +1714,11 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B52" s="11"/>
       <c r="C52" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D52" s="10"/>
       <c r="E52">
@@ -1735,8 +1732,8 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A41:A1048576 A2:A39" xr:uid="{12928F6E-5312-4F47-8E2A-2DA233330493}">
-      <formula1>"Building,Gate,Roadside,Residential,Infrastructure,Facilities,Car park"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{1206F71A-1E02-4C3E-A41A-3C6D684B1E81}">
+      <formula1>"Building,Gate,Roadside,Infrastructure,Facilities,Car park"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>

</xml_diff>